<commit_message>
added new media information to all files
</commit_message>
<xml_diff>
--- a/results/cross_table_per_100_million_tokens_rounded.xlsx
+++ b/results/cross_table_per_100_million_tokens_rounded.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Mijn Drive\Studie informatiekunde\master\master project\project\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{989D1CD1-DAFC-43E8-BBE3-29ADD89A7292}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91787CA3-94CD-4D16-AE7D-ED1A817F8059}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5A7434B7-1035-4331-815A-FB1FAF449086}"/>
   </bookViews>
@@ -678,14 +678,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="255" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -732,10 +739,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8B00A6EE-87B6-420A-9ABD-09E9B68A31D7}" name="cross_table_per_100_million_tokens_rounded" displayName="cross_table_per_100_million_tokens_rounded" ref="A1:T183" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:T183" xr:uid="{F682CB98-69A8-4AB8-B4BE-50EB277CD528}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8B00A6EE-87B6-420A-9ABD-09E9B68A31D7}" name="cross_table_per_100_million_tokens_rounded" displayName="cross_table_per_100_million_tokens_rounded" ref="A1:T183" tableType="queryTable" totalsRowShown="0" headerRowDxfId="0">
   <tableColumns count="20">
-    <tableColumn id="1" xr3:uid="{0C71C6BA-BBEF-44FE-8A50-449FC1D440D4}" uniqueName="1" name="Idiom" queryTableFieldId="1" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{0C71C6BA-BBEF-44FE-8A50-449FC1D440D4}" uniqueName="1" name="Idiom" queryTableFieldId="1" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{E414B741-7AA0-48AF-9756-C0E520323AB2}" uniqueName="2" name="blogs" queryTableFieldId="2"/>
     <tableColumn id="3" xr3:uid="{D71FDD29-9508-4F63-8C38-86866763BA82}" uniqueName="3" name="books" queryTableFieldId="3"/>
     <tableColumn id="4" xr3:uid="{21550152-4A6F-44E6-8BA7-CE6C94A918EB}" uniqueName="4" name="brochures" queryTableFieldId="4"/>
@@ -1059,93 +1065,75 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D917A72F-1D3F-49F3-B0E1-76D145A82970}">
   <dimension ref="A1:T183"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="B64" sqref="B64"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="30.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="20" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:20" s="2" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="R1" t="s">
+      <c r="R1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="S1" t="s">
+      <c r="S1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="T1" t="s">
+      <c r="T1" s="2" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>